<commit_message>
update database & sample data
</commit_message>
<xml_diff>
--- a/Quiz challenge/Quiz simple data.xlsx
+++ b/Quiz challenge/Quiz simple data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Mentorship_Program\Quiz challenge\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D9C349F-3E4B-4B79-B835-A9C5FED65936}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DD2EE9C-A49D-4DD0-8845-86E7E99D5DEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{7C43A32B-1E6E-4A0B-8D6F-624FBD4948C3}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="93">
   <si>
     <t>Quiz</t>
   </si>
@@ -65,9 +65,6 @@
     <t>TopicId</t>
   </si>
   <si>
-    <t>QuestionTypeID</t>
-  </si>
-  <si>
     <t>Answer</t>
   </si>
   <si>
@@ -95,9 +92,6 @@
     <t>UserName</t>
   </si>
   <si>
-    <t>Email</t>
-  </si>
-  <si>
     <t>Password</t>
   </si>
   <si>
@@ -182,9 +176,6 @@
     <t xml:space="preserve">FreeText </t>
   </si>
   <si>
-    <t>Quiz C# Căn Bản</t>
-  </si>
-  <si>
     <t>Kiến thức cơ bản về C#</t>
   </si>
   <si>
@@ -227,9 +218,6 @@
     <t>Nam</t>
   </si>
   <si>
-    <t>nam@gmail.com</t>
-  </si>
-  <si>
     <t>password1</t>
   </si>
   <si>
@@ -239,17 +227,101 @@
     <t>"Sử dụng foreach để lặp qua một mảng"</t>
   </si>
   <si>
-    <t>Tạo list question</t>
-  </si>
-  <si>
-    <t>answer</t>
+    <t>UserRole</t>
+  </si>
+  <si>
+    <t>UserId</t>
+  </si>
+  <si>
+    <t>RoleId</t>
+  </si>
+  <si>
+    <t>Role</t>
+  </si>
+  <si>
+    <t>RoleName</t>
+  </si>
+  <si>
+    <t>Admin</t>
+  </si>
+  <si>
+    <t>Register</t>
+  </si>
+  <si>
+    <t>Guest</t>
+  </si>
+  <si>
+    <t>password2</t>
+  </si>
+  <si>
+    <t>password3</t>
+  </si>
+  <si>
+    <t>John</t>
+  </si>
+  <si>
+    <t>Luffy</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>TypeName</t>
+  </si>
+  <si>
+    <t>Tag</t>
+  </si>
+  <si>
+    <t>Column1</t>
+  </si>
+  <si>
+    <t>TagId</t>
+  </si>
+  <si>
+    <t>Data Structures</t>
+  </si>
+  <si>
+    <t>TypeId</t>
+  </si>
+  <si>
+    <t>QuizTag</t>
+  </si>
+  <si>
+    <t>Quick Quiz</t>
+  </si>
+  <si>
+    <t>Algorithm</t>
+  </si>
+  <si>
+    <t>C# Căn Bản</t>
+  </si>
+  <si>
+    <t>Multiple Choice</t>
+  </si>
+  <si>
+    <t>Fill in the Blank</t>
+  </si>
+  <si>
+    <t>Essay question</t>
+  </si>
+  <si>
+    <t>nam@email.com</t>
+  </si>
+  <si>
+    <t>ohn@email.com</t>
+  </si>
+  <si>
+    <t>Luffy@email.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -274,14 +346,6 @@
     </font>
     <font>
       <sz val="8"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -336,11 +400,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -372,18 +435,493 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="71">
+  <dxfs count="98">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color theme="7"/>
+        </left>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -498,25 +1036,6 @@
     <dxf>
       <font>
         <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
         <strike val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
@@ -532,63 +1051,6 @@
     </dxf>
     <dxf>
       <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
         <b/>
         <strike val="0"/>
         <outline val="0"/>
@@ -604,11 +1066,61 @@
       <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <border outline="0">
-        <left style="thin">
-          <color theme="7"/>
-        </left>
-      </border>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -640,6 +1152,22 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
       <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -736,64 +1264,10 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
       <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
         <b/>
         <strike val="0"/>
         <outline val="0"/>
@@ -809,11 +1283,42 @@
       <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <border outline="0">
-        <left style="thin">
-          <color theme="7"/>
-        </left>
-      </border>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -834,6 +1339,25 @@
     <dxf>
       <font>
         <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
         <strike val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
@@ -846,63 +1370,6 @@
         <scheme val="minor"/>
       </font>
       <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1126,25 +1593,6 @@
     <dxf>
       <font>
         <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
         <strike val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
@@ -1160,63 +1608,6 @@
     </dxf>
     <dxf>
       <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
         <b/>
         <strike val="0"/>
         <outline val="0"/>
@@ -1232,11 +1623,61 @@
       <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <border outline="0">
-        <left style="thin">
-          <color theme="7"/>
-        </left>
-      </border>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1272,44 +1713,6 @@
     </dxf>
     <dxf>
       <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
         <b/>
         <strike val="0"/>
         <outline val="0"/>
@@ -1325,11 +1728,42 @@
       <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <border outline="0">
-        <left style="thin">
-          <color theme="7"/>
-        </left>
-      </border>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1346,6 +1780,25 @@
         <scheme val="minor"/>
       </font>
       <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1494,6 +1947,136 @@
       </border>
     </dxf>
     <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <border outline="0">
         <left style="thin">
           <color theme="7"/>
@@ -1501,169 +2084,60 @@
       </border>
     </dxf>
     <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border outline="0">
+        <left style="thin">
+          <color theme="7"/>
+        </left>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color theme="7"/>
+        </left>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color theme="7"/>
+        </left>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color theme="7"/>
+        </left>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color theme="7"/>
+        </left>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color theme="7"/>
+        </left>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color theme="7"/>
+        </left>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color theme="7"/>
+        </left>
+      </border>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1679,136 +2153,193 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0A79962B-AEC1-4BA2-8BBE-60DA57A5CFBD}" name="Table1" displayName="Table1" ref="A2:E5" totalsRowShown="0" headerRowDxfId="70" dataDxfId="69">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0A79962B-AEC1-4BA2-8BBE-60DA57A5CFBD}" name="Table1" displayName="Table1" ref="A2:E5" totalsRowShown="0" headerRowDxfId="83" dataDxfId="82">
   <autoFilter ref="A2:E5" xr:uid="{0A79962B-AEC1-4BA2-8BBE-60DA57A5CFBD}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{F238FED4-8AD9-415E-BF00-9C7B319C1400}" name="Id" dataDxfId="68"/>
-    <tableColumn id="2" xr3:uid="{E0D6CABF-B5D0-4825-9E10-24C9F93DB042}" name="Title" dataDxfId="67"/>
-    <tableColumn id="3" xr3:uid="{6B319D20-A60B-4504-9908-A8CF0C774521}" name="Description" dataDxfId="66"/>
-    <tableColumn id="4" xr3:uid="{AB97B883-C760-4355-97E9-1D0BC51D23A3}" name="CreatedAt" dataDxfId="65"/>
-    <tableColumn id="5" xr3:uid="{773CB633-5043-4D94-8C79-DA10214C4278}" name="TimeLimit" dataDxfId="64"/>
+    <tableColumn id="1" xr3:uid="{F238FED4-8AD9-415E-BF00-9C7B319C1400}" name="Id" dataDxfId="88"/>
+    <tableColumn id="2" xr3:uid="{E0D6CABF-B5D0-4825-9E10-24C9F93DB042}" name="Title" dataDxfId="87"/>
+    <tableColumn id="3" xr3:uid="{6B319D20-A60B-4504-9908-A8CF0C774521}" name="Description" dataDxfId="86"/>
+    <tableColumn id="4" xr3:uid="{AB97B883-C760-4355-97E9-1D0BC51D23A3}" name="CreatedAt" dataDxfId="85"/>
+    <tableColumn id="5" xr3:uid="{773CB633-5043-4D94-8C79-DA10214C4278}" name="TimeLimit" dataDxfId="84"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight19" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{AEB1B0AB-8A75-404F-AC46-C9C83A408145}" name="Table4116" displayName="Table4116" ref="G26:K29" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{AEB1B0AB-8A75-404F-AC46-C9C83A408145}" name="Table4116" displayName="Table4116" ref="G26:K29" totalsRowShown="0" headerRowDxfId="27" dataDxfId="26">
   <autoFilter ref="G26:K29" xr:uid="{AEB1B0AB-8A75-404F-AC46-C9C83A408145}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{F53C790D-B82B-4BAF-8ED9-8E9B5E30319B}" name="Id" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{56133213-8380-4969-A3B5-7B121D24AC10}" name="UserQuizId " dataDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{939056A5-287C-41B8-AD54-CC6B7E027FE8}" name="QuestionId " dataDxfId="2"/>
-    <tableColumn id="4" xr3:uid="{54E8C5D0-0929-4C3C-BBFE-434E783DC4F0}" name="AnswerId " dataDxfId="1"/>
-    <tableColumn id="5" xr3:uid="{CA923F4E-9135-4650-820C-838E8B063852}" name="FreeText " dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{F53C790D-B82B-4BAF-8ED9-8E9B5E30319B}" name="Id" dataDxfId="32"/>
+    <tableColumn id="2" xr3:uid="{56133213-8380-4969-A3B5-7B121D24AC10}" name="UserQuizId " dataDxfId="31"/>
+    <tableColumn id="3" xr3:uid="{939056A5-287C-41B8-AD54-CC6B7E027FE8}" name="QuestionId " dataDxfId="30"/>
+    <tableColumn id="4" xr3:uid="{54E8C5D0-0929-4C3C-BBFE-434E783DC4F0}" name="AnswerId " dataDxfId="29"/>
+    <tableColumn id="5" xr3:uid="{CA923F4E-9135-4650-820C-838E8B063852}" name="FreeText " dataDxfId="28"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight19" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{5EF00002-90ED-499C-A6B7-295B92CCAD08}" name="Table791339" displayName="Table791339" ref="H20:J23" totalsRowShown="0" headerRowDxfId="22" dataDxfId="21" tableBorderDxfId="92">
+  <autoFilter ref="H20:J23" xr:uid="{5EF00002-90ED-499C-A6B7-295B92CCAD08}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{95A5F424-E322-4E19-BD04-574E4757D985}" name="Id" dataDxfId="25"/>
+    <tableColumn id="2" xr3:uid="{F47EAF99-A848-4F78-B3CF-8B338BCC4322}" name="UserId" dataDxfId="24"/>
+    <tableColumn id="3" xr3:uid="{8E39D621-8D60-49C1-9B93-416027E720CC}" name="RoleId" dataDxfId="23"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight19" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{3F1D2D8D-F15C-44EF-A0DC-AADD7EB5D9DD}" name="Table79133914" displayName="Table79133914" ref="J14:K17" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17" tableBorderDxfId="91">
+  <autoFilter ref="J14:K17" xr:uid="{3F1D2D8D-F15C-44EF-A0DC-AADD7EB5D9DD}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{C6F3F560-D724-4DE4-ABDC-739035A53B46}" name="Id" dataDxfId="20"/>
+    <tableColumn id="2" xr3:uid="{8305E703-F7D3-4F2F-BBAD-2F1F7B3FF6CD}" name="RoleName" dataDxfId="19"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight19" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{758FCF58-11CF-4F6E-BB37-CBCB4FDD9179}" name="Table7913391415" displayName="Table7913391415" ref="M14:N17" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15" tableBorderDxfId="90">
+  <autoFilter ref="M14:N17" xr:uid="{758FCF58-11CF-4F6E-BB37-CBCB4FDD9179}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{C2533080-054E-44EF-A66B-1FF609F85487}" name="Id" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{7AE9E73D-B773-4753-A6F3-9EF8AF42E6CE}" name="TypeName" dataDxfId="3"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight19" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{E20F82DB-463C-45EB-86AA-455A74ECDFCB}" name="Table791339141516" displayName="Table791339141516" ref="K8:L11" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11" tableBorderDxfId="89">
+  <autoFilter ref="K8:L11" xr:uid="{E20F82DB-463C-45EB-86AA-455A74ECDFCB}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{C7A1C32B-C429-4703-A9AA-39EC009955C1}" name="Id" dataDxfId="14"/>
+    <tableColumn id="2" xr3:uid="{7A920786-0E2D-4329-81AA-1DAE95E5D364}" name="TypeName" dataDxfId="13"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight19" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{946485ED-02FC-46A8-8EF9-800E43C9FAA1}" name="Table7913317" displayName="Table7913317" ref="N8:P11" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9" tableBorderDxfId="8">
+  <autoFilter ref="N8:P11" xr:uid="{946485ED-02FC-46A8-8EF9-800E43C9FAA1}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{FB3FB424-4531-48FD-A206-D2957E2A26B0}" name="Id" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{0A967AD0-0A48-4A60-B1C6-C853FCAEC469}" name="QuizId" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{F5E411F8-4FC0-4725-943A-733B504B7A16}" name="TagId" dataDxfId="5"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight19" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{B9237A2E-255C-4FAC-BE16-9DC8EE8ED36E}" name="Table3" displayName="Table3" ref="G2:L5" totalsRowShown="0" headerRowDxfId="63" dataDxfId="62" tableBorderDxfId="61">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{B9237A2E-255C-4FAC-BE16-9DC8EE8ED36E}" name="Table3" displayName="Table3" ref="G2:L5" totalsRowShown="0" headerRowDxfId="75" dataDxfId="74" tableBorderDxfId="97">
   <autoFilter ref="G2:L5" xr:uid="{B9237A2E-255C-4FAC-BE16-9DC8EE8ED36E}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{11A3F043-76AA-497A-8E70-04B4EEFC231A}" name="Id" dataDxfId="60"/>
-    <tableColumn id="2" xr3:uid="{D440EAB9-2CA3-43CA-9FA6-D491B473723D}" name="Content" dataDxfId="59"/>
-    <tableColumn id="3" xr3:uid="{B76291C2-CD8B-4555-83B5-1C9882F49F3C}" name="Format" dataDxfId="58"/>
-    <tableColumn id="4" xr3:uid="{86322B2A-4305-45A0-80DA-5F1A034A190A}" name="LevelId" dataDxfId="57"/>
-    <tableColumn id="5" xr3:uid="{7FAC9DF3-7A40-4212-B353-A4F4CE9CCB6F}" name="TopicId" dataDxfId="56"/>
-    <tableColumn id="6" xr3:uid="{E1D4D179-9F5D-466C-B4DF-CFA76EAEB4B7}" name="QuestionTypeID" dataDxfId="55"/>
+    <tableColumn id="1" xr3:uid="{11A3F043-76AA-497A-8E70-04B4EEFC231A}" name="Id" dataDxfId="81"/>
+    <tableColumn id="2" xr3:uid="{D440EAB9-2CA3-43CA-9FA6-D491B473723D}" name="Content" dataDxfId="80"/>
+    <tableColumn id="3" xr3:uid="{B76291C2-CD8B-4555-83B5-1C9882F49F3C}" name="Format" dataDxfId="79"/>
+    <tableColumn id="4" xr3:uid="{86322B2A-4305-45A0-80DA-5F1A034A190A}" name="LevelId" dataDxfId="78"/>
+    <tableColumn id="5" xr3:uid="{7FAC9DF3-7A40-4212-B353-A4F4CE9CCB6F}" name="TopicId" dataDxfId="77"/>
+    <tableColumn id="6" xr3:uid="{E1D4D179-9F5D-466C-B4DF-CFA76EAEB4B7}" name="TypeId" dataDxfId="76"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight19" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{D07F7F1F-0C11-4420-86ED-32ADFC35D176}" name="Table6" displayName="Table6" ref="A14:C17" totalsRowShown="0" headerRowDxfId="54" dataDxfId="53" tableBorderDxfId="52">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{D07F7F1F-0C11-4420-86ED-32ADFC35D176}" name="Table6" displayName="Table6" ref="A14:C17" totalsRowShown="0" headerRowDxfId="70" dataDxfId="69" tableBorderDxfId="96">
   <autoFilter ref="A14:C17" xr:uid="{D07F7F1F-0C11-4420-86ED-32ADFC35D176}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{9C6E43C9-D9C3-4FF2-B9D8-AF875E68B807}" name="Id" dataDxfId="51"/>
-    <tableColumn id="2" xr3:uid="{2FF6299F-DC71-4BD0-AB90-FAAD1B4B5A53}" name="Name" dataDxfId="50"/>
-    <tableColumn id="3" xr3:uid="{ABC80DC0-4DAE-40AC-AF3F-0A7147347D49}" name="ParentTopicID" dataDxfId="49"/>
+    <tableColumn id="1" xr3:uid="{9C6E43C9-D9C3-4FF2-B9D8-AF875E68B807}" name="Id" dataDxfId="73"/>
+    <tableColumn id="2" xr3:uid="{2FF6299F-DC71-4BD0-AB90-FAAD1B4B5A53}" name="Name" dataDxfId="72"/>
+    <tableColumn id="3" xr3:uid="{ABC80DC0-4DAE-40AC-AF3F-0A7147347D49}" name="ParentTopicID" dataDxfId="71"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight19" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{09B70181-5D84-477D-BD87-E795B37276C4}" name="Table7" displayName="Table7" ref="E14:H17" totalsRowShown="0" headerRowDxfId="48" dataDxfId="47" tableBorderDxfId="46">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{09B70181-5D84-477D-BD87-E795B37276C4}" name="Table7" displayName="Table7" ref="E14:H17" totalsRowShown="0" headerRowDxfId="64" dataDxfId="63" tableBorderDxfId="95">
   <autoFilter ref="E14:H17" xr:uid="{09B70181-5D84-477D-BD87-E795B37276C4}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{328F0973-54AB-4F4E-B9DF-38A92B7D0EB7}" name="Id" dataDxfId="45"/>
-    <tableColumn id="2" xr3:uid="{D0E3492C-A244-453E-ADF6-AC2921F6BE53}" name="LevelName" dataDxfId="44"/>
-    <tableColumn id="4" xr3:uid="{32553B2B-51C8-4027-B7F6-F78571A9A039}" name="ScoreWeight" dataDxfId="43"/>
-    <tableColumn id="5" xr3:uid="{144C7DD5-B5F0-445F-9D2E-440C8ABE9A42}" name="TimeConstraint" dataDxfId="42"/>
+    <tableColumn id="1" xr3:uid="{328F0973-54AB-4F4E-B9DF-38A92B7D0EB7}" name="Id" dataDxfId="68"/>
+    <tableColumn id="2" xr3:uid="{D0E3492C-A244-453E-ADF6-AC2921F6BE53}" name="LevelName" dataDxfId="67"/>
+    <tableColumn id="4" xr3:uid="{32553B2B-51C8-4027-B7F6-F78571A9A039}" name="ScoreWeight" dataDxfId="66"/>
+    <tableColumn id="5" xr3:uid="{144C7DD5-B5F0-445F-9D2E-440C8ABE9A42}" name="TimeConstraint" dataDxfId="65"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight19" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{B2773DDF-A39C-44D7-AEDC-CF8D980FB8FF}" name="Table411" displayName="Table411" ref="A26:E29" totalsRowShown="0" headerRowDxfId="41" dataDxfId="40">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{B2773DDF-A39C-44D7-AEDC-CF8D980FB8FF}" name="Table411" displayName="Table411" ref="A26:E29" totalsRowShown="0" headerRowDxfId="57" dataDxfId="56">
   <autoFilter ref="A26:E29" xr:uid="{B2773DDF-A39C-44D7-AEDC-CF8D980FB8FF}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{BA579B0D-99C8-4846-AA2A-58710BEE3F30}" name="Id" dataDxfId="39"/>
-    <tableColumn id="2" xr3:uid="{F494C43B-BA5A-40CF-A7AE-537CD9375379}" name="UserID" dataDxfId="38"/>
-    <tableColumn id="3" xr3:uid="{68945211-9457-454C-A551-79DA66D3771B}" name="QuizID" dataDxfId="37"/>
-    <tableColumn id="4" xr3:uid="{A68FFC5C-3CC3-4441-9453-7E98D5CC6602}" name="CompletionTime" dataDxfId="36"/>
-    <tableColumn id="5" xr3:uid="{F002231A-EC2F-48C4-A011-265F516024DA}" name="AttemptAt" dataDxfId="35"/>
+    <tableColumn id="1" xr3:uid="{BA579B0D-99C8-4846-AA2A-58710BEE3F30}" name="Id" dataDxfId="62"/>
+    <tableColumn id="2" xr3:uid="{F494C43B-BA5A-40CF-A7AE-537CD9375379}" name="UserID" dataDxfId="61"/>
+    <tableColumn id="3" xr3:uid="{68945211-9457-454C-A551-79DA66D3771B}" name="QuizID" dataDxfId="60"/>
+    <tableColumn id="4" xr3:uid="{A68FFC5C-3CC3-4441-9453-7E98D5CC6602}" name="CompletionTime" dataDxfId="59"/>
+    <tableColumn id="5" xr3:uid="{F002231A-EC2F-48C4-A011-265F516024DA}" name="AttemptAt" dataDxfId="58"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight19" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{42F24B4A-E5FC-4580-AC79-7A87B6E74532}" name="Table41012" displayName="Table41012" ref="A20:F23" totalsRowShown="0" headerRowDxfId="34" dataDxfId="33">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{42F24B4A-E5FC-4580-AC79-7A87B6E74532}" name="Table41012" displayName="Table41012" ref="A20:F23" totalsRowShown="0" headerRowDxfId="52" dataDxfId="51">
   <autoFilter ref="A20:F23" xr:uid="{42F24B4A-E5FC-4580-AC79-7A87B6E74532}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{AB2F2B92-4F5E-45D5-94FB-ADB8435B9566}" name="Id" dataDxfId="32"/>
-    <tableColumn id="2" xr3:uid="{B9827B33-45BE-47C1-A171-29F23AD74DC2}" name="UserName" dataDxfId="31"/>
-    <tableColumn id="3" xr3:uid="{598DE96A-8525-495C-8324-9A1B70055E97}" name="Email" dataDxfId="30"/>
-    <tableColumn id="4" xr3:uid="{D74DA2E3-95DA-43B1-B28C-B64A14ABA8B1}" name="Password" dataDxfId="29"/>
-    <tableColumn id="5" xr3:uid="{61E76584-885D-4BCA-A61B-05EE3807BA29}" name="CreatedAt" dataDxfId="28"/>
-    <tableColumn id="6" xr3:uid="{C5B91E7E-7207-4164-A092-76CF2F672774}" name="UpdateAt" dataDxfId="27"/>
+    <tableColumn id="1" xr3:uid="{AB2F2B92-4F5E-45D5-94FB-ADB8435B9566}" name="Id" dataDxfId="55"/>
+    <tableColumn id="2" xr3:uid="{B9827B33-45BE-47C1-A171-29F23AD74DC2}" name="UserName" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{B49FE75E-62B6-4D37-8C90-5095A776B904}" name="Column1" dataDxfId="0"/>
+    <tableColumn id="4" xr3:uid="{D74DA2E3-95DA-43B1-B28C-B64A14ABA8B1}" name="Password" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{61E76584-885D-4BCA-A61B-05EE3807BA29}" name="CreatedAt" dataDxfId="54"/>
+    <tableColumn id="6" xr3:uid="{C5B91E7E-7207-4164-A092-76CF2F672774}" name="UpdateAt" dataDxfId="53"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight19" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{0A3741F9-7340-4634-958D-243B2CB30081}" name="Table79133" displayName="Table79133" ref="G8:I11" totalsRowShown="0" headerRowDxfId="26" dataDxfId="25" tableBorderDxfId="24">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{0A3741F9-7340-4634-958D-243B2CB30081}" name="Table79133" displayName="Table79133" ref="G8:I11" totalsRowShown="0" headerRowDxfId="47" dataDxfId="46" tableBorderDxfId="94">
   <autoFilter ref="G8:I11" xr:uid="{0A3741F9-7340-4634-958D-243B2CB30081}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{31F14D34-66D8-41C0-A3EA-4754B439DA63}" name="Id" dataDxfId="23"/>
-    <tableColumn id="2" xr3:uid="{8E3A139A-5007-4A16-BB0C-C46739F67B30}" name="QuestionId" dataDxfId="22"/>
-    <tableColumn id="3" xr3:uid="{F32C6264-78B0-42EF-820B-362961B4B35B}" name="AnswerId" dataDxfId="21"/>
+    <tableColumn id="1" xr3:uid="{31F14D34-66D8-41C0-A3EA-4754B439DA63}" name="Id" dataDxfId="50"/>
+    <tableColumn id="2" xr3:uid="{8E3A139A-5007-4A16-BB0C-C46739F67B30}" name="QuestionId" dataDxfId="49"/>
+    <tableColumn id="3" xr3:uid="{F32C6264-78B0-42EF-820B-362961B4B35B}" name="AnswerId" dataDxfId="48"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight19" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{1FA08D23-38C9-4F9D-A38F-2FAD175CEAC5}" name="Table4" displayName="Table4" ref="A8:E11" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{1FA08D23-38C9-4F9D-A38F-2FAD175CEAC5}" name="Table4" displayName="Table4" ref="A8:E11" totalsRowShown="0" headerRowDxfId="40" dataDxfId="39">
   <autoFilter ref="A8:E11" xr:uid="{1FA08D23-38C9-4F9D-A38F-2FAD175CEAC5}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{6D940C02-9530-4EAD-9CFB-AEBCF3BB6A31}" name="Id" dataDxfId="18"/>
-    <tableColumn id="2" xr3:uid="{12869B36-21EC-4622-8455-75F60E2AD58B}" name="AnswerText" dataDxfId="17"/>
-    <tableColumn id="4" xr3:uid="{97B8C5D1-BBA2-4E43-902B-8228BD6EFBA7}" name="IsCorrect" dataDxfId="16"/>
-    <tableColumn id="5" xr3:uid="{415B0A9F-E9AC-4B8E-9FF6-5F36248C5433}" name="IsDynamic" dataDxfId="15"/>
-    <tableColumn id="3" xr3:uid="{13FBD282-3F29-4BAF-BB02-64422CAE2315}" name="CanBeSuggested" dataDxfId="14"/>
+    <tableColumn id="1" xr3:uid="{6D940C02-9530-4EAD-9CFB-AEBCF3BB6A31}" name="Id" dataDxfId="45"/>
+    <tableColumn id="2" xr3:uid="{12869B36-21EC-4622-8455-75F60E2AD58B}" name="AnswerText" dataDxfId="44"/>
+    <tableColumn id="4" xr3:uid="{97B8C5D1-BBA2-4E43-902B-8228BD6EFBA7}" name="IsCorrect" dataDxfId="43"/>
+    <tableColumn id="5" xr3:uid="{415B0A9F-E9AC-4B8E-9FF6-5F36248C5433}" name="IsDynamic" dataDxfId="42"/>
+    <tableColumn id="3" xr3:uid="{13FBD282-3F29-4BAF-BB02-64422CAE2315}" name="CanBeSuggested" dataDxfId="41"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight19" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{BCABB276-88BA-4F24-A0D9-15F6C263304F}" name="Table61410" displayName="Table61410" ref="N2:Q5" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12" tableBorderDxfId="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{BCABB276-88BA-4F24-A0D9-15F6C263304F}" name="Table61410" displayName="Table61410" ref="N2:Q5" totalsRowShown="0" headerRowDxfId="34" dataDxfId="33" tableBorderDxfId="93">
   <autoFilter ref="N2:Q5" xr:uid="{BCABB276-88BA-4F24-A0D9-15F6C263304F}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{5EB3FF8F-A636-4EEE-B8E1-1807AA06E054}" name="Id" dataDxfId="10"/>
-    <tableColumn id="2" xr3:uid="{CEAAA849-0E1B-4880-BB0D-7B68048D946C}" name="QuizId" dataDxfId="9"/>
-    <tableColumn id="3" xr3:uid="{DAED52E6-0B97-493B-8C38-2D2C83FDE3CC}" name="QuestionId" dataDxfId="8"/>
-    <tableColumn id="4" xr3:uid="{1B02BC0F-6221-4E41-A04C-917A41872E22}" name="Order" dataDxfId="7"/>
+    <tableColumn id="1" xr3:uid="{5EB3FF8F-A636-4EEE-B8E1-1807AA06E054}" name="Id" dataDxfId="38"/>
+    <tableColumn id="2" xr3:uid="{CEAAA849-0E1B-4880-BB0D-7B68048D946C}" name="QuizId" dataDxfId="37"/>
+    <tableColumn id="3" xr3:uid="{DAED52E6-0B97-493B-8C38-2D2C83FDE3CC}" name="QuestionId" dataDxfId="36"/>
+    <tableColumn id="4" xr3:uid="{1B02BC0F-6221-4E41-A04C-917A41872E22}" name="Order" dataDxfId="35"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight19" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2133,8 +2664,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90A88412-2F2D-4255-B565-F6FDBB99DF9D}">
   <dimension ref="A1:Q29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="M16" sqref="M16"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="N21" sqref="N21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.3"/>
@@ -2143,18 +2674,18 @@
     <col min="2" max="2" width="11.44140625" style="1" customWidth="1"/>
     <col min="3" max="3" width="11.77734375" style="1" customWidth="1"/>
     <col min="4" max="4" width="11.33203125" style="1" customWidth="1"/>
-    <col min="5" max="6" width="12.109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="12.109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="9.88671875" style="1" customWidth="1"/>
     <col min="7" max="7" width="11.109375" style="1" customWidth="1"/>
     <col min="8" max="8" width="12.109375" style="1" customWidth="1"/>
     <col min="9" max="9" width="9.5546875" style="1" customWidth="1"/>
     <col min="10" max="10" width="10.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.77734375" style="1" customWidth="1"/>
+    <col min="11" max="11" width="9.21875" style="1" customWidth="1"/>
     <col min="12" max="12" width="11.44140625" style="1" customWidth="1"/>
-    <col min="13" max="13" width="12.33203125" style="1" customWidth="1"/>
+    <col min="13" max="13" width="9.5546875" style="1" customWidth="1"/>
     <col min="14" max="14" width="8.88671875" style="1"/>
     <col min="15" max="15" width="11" style="1" customWidth="1"/>
-    <col min="16" max="16" width="13.109375" style="1" customWidth="1"/>
-    <col min="17" max="17" width="11.6640625" style="1" customWidth="1"/>
+    <col min="16" max="17" width="11.6640625" style="1" customWidth="1"/>
     <col min="18" max="18" width="8.88671875" style="1" customWidth="1"/>
     <col min="19" max="16384" width="8.88671875" style="1"/>
   </cols>
@@ -2167,7 +2698,7 @@
         <v>4</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:17" ht="12.6" thickBot="1" x14ac:dyDescent="0.35">
@@ -2181,10 +2712,10 @@
         <v>1</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>2</v>
@@ -2202,30 +2733,30 @@
         <v>8</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>9</v>
+        <v>81</v>
       </c>
       <c r="N2" s="4" t="s">
         <v>2</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="Q2" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="C3" t="s">
-        <v>49</v>
+        <v>85</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>46</v>
       </c>
       <c r="D3" s="9">
         <v>45590</v>
@@ -2237,10 +2768,10 @@
         <v>1</v>
       </c>
       <c r="H3" s="10" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="J3" s="2">
         <v>1</v>
@@ -2276,10 +2807,10 @@
         <v>2</v>
       </c>
       <c r="H4" s="10" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="J4" s="2">
         <v>1</v>
@@ -2315,10 +2846,10 @@
         <v>3</v>
       </c>
       <c r="H5" s="10" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="J5" s="2">
         <v>2</v>
@@ -2344,37 +2875,59 @@
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H7" s="5"/>
+      <c r="K7" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="N7" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="O7" s="5"/>
     </row>
     <row r="8" spans="1:17" ht="12.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="D8" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="1" t="s">
-        <v>13</v>
-      </c>
       <c r="E8" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="G8" s="4" t="s">
         <v>2</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
+      </c>
+      <c r="K8" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="N8" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="O8" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="P8" s="1" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.3">
@@ -2382,7 +2935,7 @@
         <v>1</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C9" s="2">
         <v>1</v>
@@ -2403,19 +2956,29 @@
       <c r="I9" s="2">
         <v>1</v>
       </c>
-      <c r="L9" s="2" t="s">
-        <v>67</v>
+      <c r="K9" s="7">
+        <v>1</v>
+      </c>
+      <c r="L9" s="10" t="s">
+        <v>80</v>
       </c>
       <c r="M9" s="2"/>
-      <c r="N9" s="2"/>
-      <c r="O9" s="2"/>
+      <c r="N9" s="7">
+        <v>1</v>
+      </c>
+      <c r="O9" s="2">
+        <v>1</v>
+      </c>
+      <c r="P9" s="2">
+        <v>2</v>
+      </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A10" s="6">
         <v>2</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C10" s="2">
         <v>0</v>
@@ -2436,19 +2999,25 @@
       <c r="I10" s="2">
         <v>2</v>
       </c>
-      <c r="L10" s="2" t="s">
-        <v>68</v>
+      <c r="K10" s="8">
+        <v>2</v>
+      </c>
+      <c r="L10" s="10" t="s">
+        <v>83</v>
       </c>
       <c r="M10" s="2"/>
-      <c r="N10" s="2"/>
+      <c r="N10" s="8">
+        <v>2</v>
+      </c>
       <c r="O10" s="2"/>
+      <c r="P10" s="2"/>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A11" s="6">
         <v>3</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C11" s="2">
         <v>1</v>
@@ -2469,10 +3038,18 @@
       <c r="I11" s="2">
         <v>3</v>
       </c>
-      <c r="L11" s="2"/>
+      <c r="K11" s="7">
+        <v>3</v>
+      </c>
+      <c r="L11" s="10" t="s">
+        <v>84</v>
+      </c>
       <c r="M11" s="2"/>
-      <c r="N11" s="2"/>
+      <c r="N11" s="7">
+        <v>3</v>
+      </c>
       <c r="O11" s="2"/>
+      <c r="P11" s="2"/>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="L12" s="2"/>
@@ -2480,43 +3057,61 @@
       <c r="N12" s="2"/>
       <c r="O12" s="2"/>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E13" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E13" s="1" t="s">
-        <v>15</v>
-      </c>
+      <c r="J13" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="K13" s="5"/>
       <c r="L13" s="2"/>
-      <c r="M13" s="2"/>
-      <c r="N13" s="2"/>
+      <c r="M13" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="N13" s="5"/>
       <c r="O13" s="2"/>
+      <c r="P13" s="14"/>
+      <c r="Q13" s="13"/>
     </row>
     <row r="14" spans="1:17" ht="12.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="4" t="s">
         <v>2</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E14" s="4" t="s">
         <v>2</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
+      </c>
+      <c r="J14" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>67</v>
       </c>
       <c r="L14" s="2"/>
-      <c r="M14" s="2"/>
-      <c r="N14" s="2"/>
+      <c r="M14" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="N14" s="1" t="s">
+        <v>76</v>
+      </c>
       <c r="O14" s="2"/>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.3">
@@ -2524,16 +3119,16 @@
         <v>1</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="E15" s="7">
         <v>1</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="G15" s="2">
         <v>0.25</v>
@@ -2541,9 +3136,19 @@
       <c r="H15" s="2">
         <v>1</v>
       </c>
+      <c r="J15" s="7">
+        <v>1</v>
+      </c>
+      <c r="K15" s="2" t="s">
+        <v>68</v>
+      </c>
       <c r="L15" s="2"/>
-      <c r="M15" s="2"/>
-      <c r="N15" s="2"/>
+      <c r="M15" s="7">
+        <v>1</v>
+      </c>
+      <c r="N15" s="10" t="s">
+        <v>86</v>
+      </c>
       <c r="O15" s="2"/>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.3">
@@ -2551,16 +3156,16 @@
         <v>2</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="E16" s="8">
         <v>2</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="G16" s="2">
         <v>0.5</v>
@@ -2568,13 +3173,25 @@
       <c r="H16" s="2">
         <v>5</v>
       </c>
+      <c r="J16" s="8">
+        <v>2</v>
+      </c>
+      <c r="K16" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="M16" s="8">
+        <v>2</v>
+      </c>
+      <c r="N16" s="10" t="s">
+        <v>87</v>
+      </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A17" s="7">
         <v>3</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C17" s="2">
         <v>1</v>
@@ -2583,7 +3200,7 @@
         <v>3</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="G17" s="2">
         <v>1</v>
@@ -2591,44 +3208,76 @@
       <c r="H17" s="2">
         <v>10</v>
       </c>
+      <c r="J17" s="7">
+        <v>3</v>
+      </c>
+      <c r="K17" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="M17" s="7">
+        <v>3</v>
+      </c>
+      <c r="N17" s="10" t="s">
+        <v>88</v>
+      </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H19" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="I19" s="5"/>
+      <c r="O19" s="12"/>
+      <c r="P19" s="12"/>
+    </row>
+    <row r="20" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B20" s="1" t="s">
         <v>17</v>
       </c>
+      <c r="C20" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H20" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="M20" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="O20" s="12"/>
+      <c r="P20" s="12"/>
     </row>
-    <row r="20" spans="1:11" ht="12.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A21" s="7">
         <v>1</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="C21" s="11" t="s">
-        <v>63</v>
+        <v>59</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>89</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="E21" s="9">
         <v>45566</v>
@@ -2636,70 +3285,121 @@
       <c r="F21" s="9">
         <v>45566</v>
       </c>
+      <c r="H21" s="7">
+        <v>1</v>
+      </c>
+      <c r="I21" s="2">
+        <v>1</v>
+      </c>
+      <c r="J21" s="2">
+        <v>1</v>
+      </c>
+      <c r="O21" s="12"/>
+      <c r="P21" s="12"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A22" s="8">
         <v>2</v>
       </c>
-      <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
+      <c r="B22" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="E22" s="9">
+        <v>45566</v>
+      </c>
+      <c r="F22" s="9">
+        <v>45566</v>
+      </c>
+      <c r="H22" s="8">
+        <v>2</v>
+      </c>
+      <c r="I22" s="2">
+        <v>2</v>
+      </c>
+      <c r="J22" s="2">
+        <v>2</v>
+      </c>
+      <c r="O22" s="12"/>
+      <c r="P22" s="12"/>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A23" s="7">
         <v>3</v>
       </c>
-      <c r="B23" s="2"/>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
+      <c r="B23" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="E23" s="9">
+        <v>45566</v>
+      </c>
+      <c r="F23" s="9">
+        <v>45566</v>
+      </c>
+      <c r="H23" s="7">
+        <v>3</v>
+      </c>
+      <c r="I23" s="2">
+        <v>3</v>
+      </c>
+      <c r="J23" s="2">
+        <v>3</v>
+      </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A25" s="12" t="s">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A25" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B25" s="11"/>
+      <c r="G25" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="H25" s="11"/>
+    </row>
+    <row r="26" spans="1:16" ht="12.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C26" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B25" s="12"/>
-      <c r="G25" s="12" t="s">
+      <c r="D26" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G26" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="I26" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="H25" s="12"/>
+      <c r="J26" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="K26" s="1" t="s">
+        <v>45</v>
+      </c>
     </row>
-    <row r="26" spans="1:11" ht="12.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="G26" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H26" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="I26" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="J26" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="K26" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A27" s="7">
         <v>1</v>
       </c>
@@ -2728,17 +3428,25 @@
         <v>1</v>
       </c>
       <c r="K27" s="2" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A28" s="8">
         <v>2</v>
       </c>
-      <c r="B28" s="2"/>
-      <c r="C28" s="2"/>
-      <c r="D28" s="2"/>
-      <c r="E28" s="2"/>
+      <c r="B28" s="2">
+        <v>1</v>
+      </c>
+      <c r="C28" s="2">
+        <v>1</v>
+      </c>
+      <c r="D28" s="2">
+        <v>25</v>
+      </c>
+      <c r="E28" s="9">
+        <v>45591</v>
+      </c>
       <c r="G28" s="8">
         <v>2</v>
       </c>
@@ -2749,20 +3457,28 @@
         <v>2</v>
       </c>
       <c r="J28" s="2" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="K28" s="10" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A29" s="7">
         <v>3</v>
       </c>
-      <c r="B29" s="2"/>
-      <c r="C29" s="2"/>
-      <c r="D29" s="2"/>
-      <c r="E29" s="2"/>
+      <c r="B29" s="2">
+        <v>1</v>
+      </c>
+      <c r="C29" s="2">
+        <v>1</v>
+      </c>
+      <c r="D29" s="2">
+        <v>25</v>
+      </c>
+      <c r="E29" s="9">
+        <v>45592</v>
+      </c>
       <c r="G29" s="7">
         <v>3</v>
       </c>
@@ -2776,7 +3492,7 @@
         <v>3</v>
       </c>
       <c r="K29" s="2" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -2785,12 +3501,10 @@
     <mergeCell ref="G25:H25"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
-  <hyperlinks>
-    <hyperlink ref="C21" r:id="rId1" xr:uid="{C70B09A3-E467-412B-BCD9-4CFDD346099B}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="landscape" r:id="rId2"/>
-  <tableParts count="10">
+  <pageSetup orientation="landscape" r:id="rId1"/>
+  <tableParts count="15">
+    <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
     <tablePart r:id="rId4"/>
     <tablePart r:id="rId5"/>
@@ -2801,6 +3515,10 @@
     <tablePart r:id="rId10"/>
     <tablePart r:id="rId11"/>
     <tablePart r:id="rId12"/>
+    <tablePart r:id="rId13"/>
+    <tablePart r:id="rId14"/>
+    <tablePart r:id="rId15"/>
+    <tablePart r:id="rId16"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update TestCase and UseCase
</commit_message>
<xml_diff>
--- a/Quiz challenge/Quiz simple data.xlsx
+++ b/Quiz challenge/Quiz simple data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Mentorship_Program\Quiz challenge\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FCF5B0F-121C-40C4-8FC9-028CFE633785}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08E83BBB-CE61-4D7A-84F1-0A111FC9B5BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-23148" yWindow="-120" windowWidth="23256" windowHeight="12456" xr2:uid="{7C43A32B-1E6E-4A0B-8D6F-624FBD4948C3}"/>
   </bookViews>
@@ -468,63 +468,6 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1397,6 +1340,63 @@
         <scheme val="minor"/>
       </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -2245,71 +2245,71 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{AEB1B0AB-8A75-404F-AC46-C9C83A408145}" name="Table4116" displayName="Table4116" ref="A32:E35" totalsRowShown="0" headerRowDxfId="36" dataDxfId="35">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{AEB1B0AB-8A75-404F-AC46-C9C83A408145}" name="Table4116" displayName="Table4116" ref="A32:E35" totalsRowShown="0" headerRowDxfId="33" dataDxfId="32">
   <autoFilter ref="A32:E35" xr:uid="{AEB1B0AB-8A75-404F-AC46-C9C83A408145}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{F53C790D-B82B-4BAF-8ED9-8E9B5E30319B}" name="Id" dataDxfId="34"/>
-    <tableColumn id="2" xr3:uid="{56133213-8380-4969-A3B5-7B121D24AC10}" name="UserQuizId " dataDxfId="33"/>
-    <tableColumn id="3" xr3:uid="{939056A5-287C-41B8-AD54-CC6B7E027FE8}" name="QuestionId " dataDxfId="32"/>
-    <tableColumn id="4" xr3:uid="{54E8C5D0-0929-4C3C-BBFE-434E783DC4F0}" name="AnswerId " dataDxfId="31"/>
-    <tableColumn id="5" xr3:uid="{CA923F4E-9135-4650-820C-838E8B063852}" name="FreeText " dataDxfId="30"/>
+    <tableColumn id="1" xr3:uid="{F53C790D-B82B-4BAF-8ED9-8E9B5E30319B}" name="Id" dataDxfId="31"/>
+    <tableColumn id="2" xr3:uid="{56133213-8380-4969-A3B5-7B121D24AC10}" name="UserQuizId " dataDxfId="30"/>
+    <tableColumn id="3" xr3:uid="{939056A5-287C-41B8-AD54-CC6B7E027FE8}" name="QuestionId " dataDxfId="29"/>
+    <tableColumn id="4" xr3:uid="{54E8C5D0-0929-4C3C-BBFE-434E783DC4F0}" name="AnswerId " dataDxfId="28"/>
+    <tableColumn id="5" xr3:uid="{CA923F4E-9135-4650-820C-838E8B063852}" name="FreeText " dataDxfId="27"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight19" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{5EF00002-90ED-499C-A6B7-295B92CCAD08}" name="Table791339" displayName="Table791339" ref="H20:J23" totalsRowShown="0" headerRowDxfId="29" dataDxfId="28" tableBorderDxfId="27">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{5EF00002-90ED-499C-A6B7-295B92CCAD08}" name="Table791339" displayName="Table791339" ref="H20:J23" totalsRowShown="0" headerRowDxfId="26" dataDxfId="25" tableBorderDxfId="24">
   <autoFilter ref="H20:J23" xr:uid="{5EF00002-90ED-499C-A6B7-295B92CCAD08}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{95A5F424-E322-4E19-BD04-574E4757D985}" name="Id" dataDxfId="26"/>
-    <tableColumn id="2" xr3:uid="{F47EAF99-A848-4F78-B3CF-8B338BCC4322}" name="UserId" dataDxfId="25"/>
-    <tableColumn id="3" xr3:uid="{8E39D621-8D60-49C1-9B93-416027E720CC}" name="RoleId" dataDxfId="24"/>
+    <tableColumn id="1" xr3:uid="{95A5F424-E322-4E19-BD04-574E4757D985}" name="Id" dataDxfId="23"/>
+    <tableColumn id="2" xr3:uid="{F47EAF99-A848-4F78-B3CF-8B338BCC4322}" name="UserId" dataDxfId="22"/>
+    <tableColumn id="3" xr3:uid="{8E39D621-8D60-49C1-9B93-416027E720CC}" name="RoleId" dataDxfId="21"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight19" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{3F1D2D8D-F15C-44EF-A0DC-AADD7EB5D9DD}" name="Table79133914" displayName="Table79133914" ref="J14:K17" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22" tableBorderDxfId="21">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{3F1D2D8D-F15C-44EF-A0DC-AADD7EB5D9DD}" name="Table79133914" displayName="Table79133914" ref="J14:K17" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19" tableBorderDxfId="18">
   <autoFilter ref="J14:K17" xr:uid="{3F1D2D8D-F15C-44EF-A0DC-AADD7EB5D9DD}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{C6F3F560-D724-4DE4-ABDC-739035A53B46}" name="Id" dataDxfId="20"/>
-    <tableColumn id="2" xr3:uid="{8305E703-F7D3-4F2F-BBAD-2F1F7B3FF6CD}" name="RoleName" dataDxfId="19"/>
+    <tableColumn id="1" xr3:uid="{C6F3F560-D724-4DE4-ABDC-739035A53B46}" name="Id" dataDxfId="17"/>
+    <tableColumn id="2" xr3:uid="{8305E703-F7D3-4F2F-BBAD-2F1F7B3FF6CD}" name="RoleName" dataDxfId="16"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight19" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{758FCF58-11CF-4F6E-BB37-CBCB4FDD9179}" name="Table7913391415" displayName="Table7913391415" ref="M14:N17" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17" tableBorderDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{758FCF58-11CF-4F6E-BB37-CBCB4FDD9179}" name="Table7913391415" displayName="Table7913391415" ref="M14:N17" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14" tableBorderDxfId="13">
   <autoFilter ref="M14:N17" xr:uid="{758FCF58-11CF-4F6E-BB37-CBCB4FDD9179}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{C2533080-054E-44EF-A66B-1FF609F85487}" name="Id" dataDxfId="15"/>
-    <tableColumn id="2" xr3:uid="{7AE9E73D-B773-4753-A6F3-9EF8AF42E6CE}" name="TypeName" dataDxfId="14"/>
+    <tableColumn id="1" xr3:uid="{C2533080-054E-44EF-A66B-1FF609F85487}" name="Id" dataDxfId="12"/>
+    <tableColumn id="2" xr3:uid="{7AE9E73D-B773-4753-A6F3-9EF8AF42E6CE}" name="TypeName" dataDxfId="11"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight19" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{E20F82DB-463C-45EB-86AA-455A74ECDFCB}" name="Table791339141516" displayName="Table791339141516" ref="K8:L11" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12" tableBorderDxfId="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{E20F82DB-463C-45EB-86AA-455A74ECDFCB}" name="Table791339141516" displayName="Table791339141516" ref="K8:L11" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9" tableBorderDxfId="8">
   <autoFilter ref="K8:L11" xr:uid="{E20F82DB-463C-45EB-86AA-455A74ECDFCB}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{C7A1C32B-C429-4703-A9AA-39EC009955C1}" name="Id" dataDxfId="10"/>
-    <tableColumn id="2" xr3:uid="{7A920786-0E2D-4329-81AA-1DAE95E5D364}" name="TypeName" dataDxfId="9"/>
+    <tableColumn id="1" xr3:uid="{C7A1C32B-C429-4703-A9AA-39EC009955C1}" name="Id" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{7A920786-0E2D-4329-81AA-1DAE95E5D364}" name="TypeName" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight19" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{946485ED-02FC-46A8-8EF9-800E43C9FAA1}" name="Table7913317" displayName="Table7913317" ref="N8:P11" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7" tableBorderDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{946485ED-02FC-46A8-8EF9-800E43C9FAA1}" name="Table7913317" displayName="Table7913317" ref="N8:P11" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4" tableBorderDxfId="3">
   <autoFilter ref="N8:P11" xr:uid="{946485ED-02FC-46A8-8EF9-800E43C9FAA1}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{FB3FB424-4531-48FD-A206-D2957E2A26B0}" name="Id" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{0A967AD0-0A48-4A60-B1C6-C853FCAEC469}" name="QuizId" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{F5E411F8-4FC0-4725-943A-733B504B7A16}" name="TagId" dataDxfId="3"/>
+    <tableColumn id="1" xr3:uid="{FB3FB424-4531-48FD-A206-D2957E2A26B0}" name="Id" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{0A967AD0-0A48-4A60-B1C6-C853FCAEC469}" name="QuizId" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{F5E411F8-4FC0-4725-943A-733B504B7A16}" name="TagId" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight19" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2378,50 +2378,50 @@
   <autoFilter ref="A20:F23" xr:uid="{42F24B4A-E5FC-4580-AC79-7A87B6E74532}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{AB2F2B92-4F5E-45D5-94FB-ADB8435B9566}" name="Id" dataDxfId="59"/>
-    <tableColumn id="2" xr3:uid="{B9827B33-45BE-47C1-A171-29F23AD74DC2}" name="UserName" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{B49FE75E-62B6-4D37-8C90-5095A776B904}" name="Email" dataDxfId="0"/>
-    <tableColumn id="4" xr3:uid="{D74DA2E3-95DA-43B1-B28C-B64A14ABA8B1}" name="Password" dataDxfId="1"/>
-    <tableColumn id="5" xr3:uid="{61E76584-885D-4BCA-A61B-05EE3807BA29}" name="CreatedAt" dataDxfId="58"/>
-    <tableColumn id="6" xr3:uid="{C5B91E7E-7207-4164-A092-76CF2F672774}" name="UpdateAt" dataDxfId="57"/>
+    <tableColumn id="2" xr3:uid="{B9827B33-45BE-47C1-A171-29F23AD74DC2}" name="UserName" dataDxfId="58"/>
+    <tableColumn id="3" xr3:uid="{B49FE75E-62B6-4D37-8C90-5095A776B904}" name="Email" dataDxfId="57"/>
+    <tableColumn id="4" xr3:uid="{D74DA2E3-95DA-43B1-B28C-B64A14ABA8B1}" name="Password" dataDxfId="56"/>
+    <tableColumn id="5" xr3:uid="{61E76584-885D-4BCA-A61B-05EE3807BA29}" name="CreatedAt" dataDxfId="55"/>
+    <tableColumn id="6" xr3:uid="{C5B91E7E-7207-4164-A092-76CF2F672774}" name="UpdateAt" dataDxfId="54"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight19" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{0A3741F9-7340-4634-958D-243B2CB30081}" name="Table79133" displayName="Table79133" ref="G8:I11" totalsRowShown="0" headerRowDxfId="56" dataDxfId="55" tableBorderDxfId="54">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{0A3741F9-7340-4634-958D-243B2CB30081}" name="Table79133" displayName="Table79133" ref="G8:I11" totalsRowShown="0" headerRowDxfId="53" dataDxfId="52" tableBorderDxfId="51">
   <autoFilter ref="G8:I11" xr:uid="{0A3741F9-7340-4634-958D-243B2CB30081}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{31F14D34-66D8-41C0-A3EA-4754B439DA63}" name="Id" dataDxfId="53"/>
-    <tableColumn id="2" xr3:uid="{8E3A139A-5007-4A16-BB0C-C46739F67B30}" name="QuestionId" dataDxfId="52"/>
-    <tableColumn id="3" xr3:uid="{F32C6264-78B0-42EF-820B-362961B4B35B}" name="AnswerId" dataDxfId="51"/>
+    <tableColumn id="1" xr3:uid="{31F14D34-66D8-41C0-A3EA-4754B439DA63}" name="Id" dataDxfId="50"/>
+    <tableColumn id="2" xr3:uid="{8E3A139A-5007-4A16-BB0C-C46739F67B30}" name="QuestionId" dataDxfId="49"/>
+    <tableColumn id="3" xr3:uid="{F32C6264-78B0-42EF-820B-362961B4B35B}" name="AnswerId" dataDxfId="48"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight19" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{1FA08D23-38C9-4F9D-A38F-2FAD175CEAC5}" name="Table4" displayName="Table4" ref="A8:E11" totalsRowShown="0" headerRowDxfId="50" dataDxfId="49">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{1FA08D23-38C9-4F9D-A38F-2FAD175CEAC5}" name="Table4" displayName="Table4" ref="A8:E11" totalsRowShown="0" headerRowDxfId="47" dataDxfId="46">
   <autoFilter ref="A8:E11" xr:uid="{1FA08D23-38C9-4F9D-A38F-2FAD175CEAC5}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{6D940C02-9530-4EAD-9CFB-AEBCF3BB6A31}" name="Id" dataDxfId="48"/>
-    <tableColumn id="2" xr3:uid="{12869B36-21EC-4622-8455-75F60E2AD58B}" name="AnswerText" dataDxfId="47"/>
-    <tableColumn id="4" xr3:uid="{97B8C5D1-BBA2-4E43-902B-8228BD6EFBA7}" name="IsCorrect" dataDxfId="46"/>
-    <tableColumn id="5" xr3:uid="{415B0A9F-E9AC-4B8E-9FF6-5F36248C5433}" name="IsDynamic" dataDxfId="45"/>
-    <tableColumn id="3" xr3:uid="{13FBD282-3F29-4BAF-BB02-64422CAE2315}" name="CanBeSuggested" dataDxfId="44"/>
+    <tableColumn id="1" xr3:uid="{6D940C02-9530-4EAD-9CFB-AEBCF3BB6A31}" name="Id" dataDxfId="45"/>
+    <tableColumn id="2" xr3:uid="{12869B36-21EC-4622-8455-75F60E2AD58B}" name="AnswerText" dataDxfId="44"/>
+    <tableColumn id="4" xr3:uid="{97B8C5D1-BBA2-4E43-902B-8228BD6EFBA7}" name="IsCorrect" dataDxfId="43"/>
+    <tableColumn id="5" xr3:uid="{415B0A9F-E9AC-4B8E-9FF6-5F36248C5433}" name="IsDynamic" dataDxfId="42"/>
+    <tableColumn id="3" xr3:uid="{13FBD282-3F29-4BAF-BB02-64422CAE2315}" name="CanBeSuggested" dataDxfId="41"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight19" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{BCABB276-88BA-4F24-A0D9-15F6C263304F}" name="Table61410" displayName="Table61410" ref="N2:Q5" totalsRowShown="0" headerRowDxfId="43" dataDxfId="42" tableBorderDxfId="41">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{BCABB276-88BA-4F24-A0D9-15F6C263304F}" name="Table61410" displayName="Table61410" ref="N2:Q5" totalsRowShown="0" headerRowDxfId="40" dataDxfId="39" tableBorderDxfId="38">
   <autoFilter ref="N2:Q5" xr:uid="{BCABB276-88BA-4F24-A0D9-15F6C263304F}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{5EB3FF8F-A636-4EEE-B8E1-1807AA06E054}" name="Id" dataDxfId="40"/>
-    <tableColumn id="2" xr3:uid="{CEAAA849-0E1B-4880-BB0D-7B68048D946C}" name="QuizId" dataDxfId="39"/>
-    <tableColumn id="3" xr3:uid="{DAED52E6-0B97-493B-8C38-2D2C83FDE3CC}" name="QuestionId" dataDxfId="38"/>
-    <tableColumn id="4" xr3:uid="{1B02BC0F-6221-4E41-A04C-917A41872E22}" name="Order" dataDxfId="37"/>
+    <tableColumn id="1" xr3:uid="{5EB3FF8F-A636-4EEE-B8E1-1807AA06E054}" name="Id" dataDxfId="37"/>
+    <tableColumn id="2" xr3:uid="{CEAAA849-0E1B-4880-BB0D-7B68048D946C}" name="QuizId" dataDxfId="36"/>
+    <tableColumn id="3" xr3:uid="{DAED52E6-0B97-493B-8C38-2D2C83FDE3CC}" name="QuestionId" dataDxfId="35"/>
+    <tableColumn id="4" xr3:uid="{1B02BC0F-6221-4E41-A04C-917A41872E22}" name="Order" dataDxfId="34"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight19" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2746,8 +2746,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90A88412-2F2D-4255-B565-F6FDBB99DF9D}">
   <dimension ref="A1:R35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="J28" sqref="J28"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="L22" sqref="L22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12" x14ac:dyDescent="0.25"/>

</xml_diff>